<commit_message>
fixed workshop bulk tests and view
</commit_message>
<xml_diff>
--- a/registration/workshop/data/missing_cols.xlsx
+++ b/registration/workshop/data/missing_cols.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,10 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Session</t>
+          <t>SessIOn</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>facilitators</t>
         </is>
@@ -466,11 +461,6 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>description 1</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
           <t>fac1, fac11</t>
         </is>
       </c>
@@ -486,11 +476,6 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>description 2</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
           <t>fac2</t>
         </is>
       </c>
@@ -505,11 +490,6 @@
         <v>3</v>
       </c>
       <c r="C4" t="inlineStr">
-        <is>
-          <t>description 3</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
         <is>
           <t>fac3</t>
         </is>

</xml_diff>